<commit_message>
Various comments and sequence name changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -138,15 +138,6 @@
     <t>AccuracyHigh</t>
   </si>
   <si>
-    <t>QueueName</t>
-  </si>
-  <si>
-    <t>ProcessQueue</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match the two names.</t>
-  </si>
-  <si>
     <t>Transaction Successful.</t>
   </si>
   <si>
@@ -154,12 +145,48 @@
   </si>
   <si>
     <t>System exception.</t>
+  </si>
+  <si>
+    <t>fantastic</t>
+  </si>
+  <si>
+    <t>https://demo.uipath.com</t>
+  </si>
+  <si>
+    <t>KibanaDemoQueue</t>
+  </si>
+  <si>
+    <t>demo.uipath.com_credentials</t>
+  </si>
+  <si>
+    <t>OrchestratorURL</t>
+  </si>
+  <si>
+    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
+    <t>OrchestratorCredentialName</t>
+  </si>
+  <si>
+    <t>OrchestratorTenancyName</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>The URL of your orchestrator server. This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>The name of Orchestrator credentials. This should be stored in Windows Credential manager. This property is used only if you are using a Queue to store your Transaction Items.</t>
+  </si>
+  <si>
+    <t>The name of the Orchestrator tenant.  This property is used only if you are using a Queue to store your Transaction Items.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,11 +564,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,13 +591,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -580,11 +640,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +813,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -764,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -775,7 +835,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -788,7 +848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Simplified and updated README with current names of workflows.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus Cruz\Documents\GitHub\ReFrameWork\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1BF046-3B2E-4DCF-A1F2-B05AE6EDF50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
@@ -117,6 +114,10 @@
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -489,7 +490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -534,26 +537,26 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1558,9 +1561,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1604,86 +1609,86 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2665,6 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2671,7 +2675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
First commit to modern_studio branch.
Updated files to 2019.10 Studio, including changes to make them comply to most rules of the Workflow Analyzer.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus Cruz\Documents\GitHub\ReFrameWork\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1BF046-3B2E-4DCF-A1F2-B05AE6EDF50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
@@ -117,6 +114,10 @@
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -489,7 +490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -534,26 +537,26 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1558,9 +1561,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1604,86 +1609,86 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2665,6 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2671,7 +2675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>